<commit_message>
added all business logic.
</commit_message>
<xml_diff>
--- a/src/main/resources/matrix.xlsx
+++ b/src/main/resources/matrix.xlsx
@@ -8,15 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="29">
   <si>
     <t>AUD</t>
   </si>
@@ -100,6 +98,9 @@
   </si>
   <si>
     <t>NZD</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -443,7 +444,7 @@
   <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -877,7 +878,7 @@
         <v>20</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="E12" t="s">
         <v>19</v>
@@ -908,28 +909,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>